<commit_message>
feat: tlds from logs
</commit_message>
<xml_diff>
--- a/db/tlds_exclusion.xlsx
+++ b/db/tlds_exclusion.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,196 +431,1113 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>.com</t>
+          <t>.247</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>.co.uk</t>
+          <t>.72</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>.de</t>
+          <t>.ad</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>.es</t>
+          <t>.ae</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>.it</t>
+          <t>.af</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>.ru</t>
+          <t>.ag</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>.cn</t>
+          <t>.al</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>.jp</t>
+          <t>.am</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>.nl</t>
+          <t>.ao</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>.be</t>
+          <t>.at</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>.pl</t>
+          <t>.ax</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>.at</t>
+          <t>.az</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>.ch</t>
+          <t>.ba</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>.se</t>
+          <t>.bb</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>.dk</t>
+          <t>.be</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>.no</t>
+          <t>.bg</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>.fi</t>
+          <t>.biz</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>.pt</t>
+          <t>.bo</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>.gr</t>
+          <t>.br</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>.cz</t>
+          <t>.by</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>.ro</t>
+          <t>.ca</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>.hu</t>
+          <t>.cat</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>.ie</t>
+          <t>.cc</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>.org</t>
+          <t>.ch</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>.net</t>
+          <t>.city</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>.edu</t>
+          <t>.cl</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>.gov</t>
+          <t>.cn</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>.co</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>.co.in</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>.co.nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>.co.uk</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>.com.ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>.com.au</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>.com.br</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>.com.co</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>.com.mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>.com.pk</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>.com.tr</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>.com.ve</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>.cr</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>.cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>.cv</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>.cy</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>.cz</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>.de</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>.dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>.do</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>.dz</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>.ec</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>.edu</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>.ee</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>.es</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>.eu</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>.events</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>.fi</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>.fm</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>.fr</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>.frl</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>.ge</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>.gh</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>.gi</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>.gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>.gov</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>.gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>.gt</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>.hk</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>.hn</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>.hr</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>.hu</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>.id</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>.ie</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>.il</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>.in</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>.info</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>.int</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>.io</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>.ir</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>.is</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>.it</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>.jm</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>.jp</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>.ke</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>.kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>.kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>.kz</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>.lb</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>.li</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>.live</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>.lk</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>.london</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>.lt</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>.lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>.lv</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>.ly</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>.ma</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>.md</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>.media</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
           <t>.mil</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>.mk</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>.mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>.mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>.mt</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>.mx</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>.my</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>.na</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>.name</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>.net</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>.net.au</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>.news</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>.ng</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>.ni</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>.nl</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>.no</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>.np</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>.nu</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>.om</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>.online</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>.org</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>.org.uk</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>.pa</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>.pe</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>.ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>.pk</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>.pl</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>.pn</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>.pr</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>.pro</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>.ps</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>.pt</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>.py</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>.ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>.rs</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>.ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>.sa</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>.se</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>.sg</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>.si</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>.sk</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>.sm</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>.sy</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>.th</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>.today</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>.tr</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>.tt</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>.tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>.tw</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>.tz</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>.ua</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>.uahttps</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>.ug</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>.uk</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>.us</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>.uy</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>.uz</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>.ve</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>.vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>.za</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>.zw</t>
         </is>
       </c>
     </row>

</xml_diff>